<commit_message>
Added epidemics blog post; update conf data
</commit_message>
<xml_diff>
--- a/content/conference/conf_data.xlsx
+++ b/content/conference/conf_data.xlsx
@@ -1,76 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsh1702140\Documents\University\R\qleclerc\content\conference\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Washington DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modelling the World's Systems 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attended</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bristol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRF AMR Annual Conference 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charleston</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPIDEMICS 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Will attend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edinburgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microbiology Society Annual Conference 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECCMID 2020</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Conf</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>Modelling the World's Systems 2019</t>
+  </si>
+  <si>
+    <t>Attended</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>MRF AMR Annual Conference 2019</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>EPIDEMICS 2019</t>
+  </si>
+  <si>
+    <t>Will attend</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>Microbiology Society Annual Conference 2020</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>ECCMID 2020</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>May-19</t>
+  </si>
+  <si>
+    <t>Aug-19</t>
+  </si>
+  <si>
+    <t>Dec-19</t>
+  </si>
+  <si>
+    <t>Mar-20</t>
+  </si>
+  <si>
+    <t>Apr-20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -99,13 +123,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -387,14 +421,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,102 +438,120 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="n">
-        <v>38.89511</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-77.03637</v>
+      <c r="E2">
+        <v>38.895110000000003</v>
+      </c>
+      <c r="F2">
+        <v>-77.036370000000005</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="n">
-        <v>51.454514</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-2.58791</v>
+      <c r="E3">
+        <v>51.454514000000003</v>
+      </c>
+      <c r="F3">
+        <v>-2.5879099999999999</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="n">
-        <v>32.784618</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-79.940918</v>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>32.784618000000002</v>
+      </c>
+      <c r="F4">
+        <v>-79.940917999999996</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="n">
-        <v>55.953251</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-3.188267</v>
+      <c r="E5">
+        <v>55.953251000000002</v>
+      </c>
+      <c r="F5">
+        <v>-3.1882670000000002</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="n">
-        <v>48.864716</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2.349014</v>
+      <c r="E6">
+        <v>48.864716000000001</v>
+      </c>
+      <c r="F6">
+        <v>2.3490139999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added news page, updated conference
</commit_message>
<xml_diff>
--- a/content/conference/conf_data.xlsx
+++ b/content/conference/conf_data.xlsx
@@ -63,12 +63,6 @@
     <t>Microbiology Society Annual Conference 2020</t>
   </si>
   <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>ECCMID 2020</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -84,10 +78,16 @@
     <t>Mar-20</t>
   </si>
   <si>
-    <t>Apr-20</t>
-  </si>
-  <si>
     <t>EPIDEMICS7</t>
+  </si>
+  <si>
+    <t>Montpellier</t>
+  </si>
+  <si>
+    <t>EEID 2020</t>
+  </si>
+  <si>
+    <t>Jun-20</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -458,7 +458,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -478,7 +478,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -495,10 +495,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -518,7 +518,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -532,22 +532,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6">
-        <v>48.864716000000001</v>
+        <v>43.6</v>
       </c>
       <c r="F6">
-        <v>2.3490139999999999</v>
+        <v>3.8833000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update media and conferences
</commit_message>
<xml_diff>
--- a/content/conference/conf_data.xlsx
+++ b/content/conference/conf_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>City</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Bologna</t>
+  </si>
+  <si>
+    <t>Aug-21</t>
+  </si>
+  <si>
+    <t>MRF AMR Annual Conference 2021</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +536,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>51.509864999999998</v>
@@ -561,21 +567,41 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7">
+        <v>51.609864999999999</v>
+      </c>
+      <c r="F7">
+        <v>-0.21809200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
         <v>44.498955000000002</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>11.327591</v>
       </c>
     </row>

</xml_diff>